<commit_message>
Adding files for DM1092_LiPo
</commit_message>
<xml_diff>
--- a/SoMs/BW2099/BW2099_R1M1E1_IO_TABLE.xlsx
+++ b/SoMs/BW2099/BW2099_R1M1E1_IO_TABLE.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Documents\GitHub\depthai-hardware\SoMs\BW2099\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB560F9-D081-4D55-8A13-BA1B1BF111A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="3900" windowWidth="20810" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7125" yWindow="3900" windowWidth="20805" windowHeight="14430"/>
   </bookViews>
   <sheets>
     <sheet name="CONNECTOR A" sheetId="2" r:id="rId1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="290">
   <si>
     <t>Pin #</t>
   </si>
@@ -266,9 +260,6 @@
     <t>WAKEUP</t>
   </si>
   <si>
-    <t>PD: 10kR/GND</t>
-  </si>
-  <si>
     <t>COM_AUX_IO2</t>
   </si>
   <si>
@@ -566,9 +557,6 @@
     <t xml:space="preserve">SoM system reset. Leave floating if unused. </t>
   </si>
   <si>
-    <t xml:space="preserve">Leave floating.  Any SGPIO pin can be used to wake up the SoM. </t>
-  </si>
-  <si>
     <t>spi2_cs_0</t>
   </si>
   <si>
@@ -903,12 +891,15 @@
   </si>
   <si>
     <t>2099EMB_R1M1E1 INTERFACE CONNECTOR B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be pulled low with PD: 10kR/GND. Any SGPIO pin can be used to wake up the SoM. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1288,34 +1279,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.54296875" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" customWidth="1"/>
-    <col min="10" max="10" width="96.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="96.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1327,7 +1318,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1335,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -1356,10 +1347,10 @@
         <v>7</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1372,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1385,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1401,12 +1392,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" s="1"/>
       <c r="H6" s="1"/>
@@ -1414,10 +1405,10 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1432,22 +1423,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1459,7 +1450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1471,7 +1462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1486,22 +1477,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1516,22 +1507,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1543,7 +1534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1555,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1570,22 +1561,22 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1600,22 +1591,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1627,7 +1618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1639,7 +1630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1654,22 +1645,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J24" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1684,22 +1675,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1711,7 +1702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1723,7 +1714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1738,7 +1729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1746,7 +1737,7 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>44</v>
@@ -1758,7 +1749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1773,7 +1764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1787,7 +1778,7 @@
       <c r="P32" s="1"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1799,21 +1790,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
       </c>
       <c r="E34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F34" t="s">
         <v>49</v>
@@ -1831,7 +1822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1839,7 +1830,7 @@
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>55</v>
@@ -1854,7 +1845,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1862,7 +1853,7 @@
         <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D36" s="1"/>
       <c r="H36" s="1"/>
@@ -1873,7 +1864,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1881,7 +1872,7 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37" s="1"/>
       <c r="H37" t="s">
@@ -1894,15 +1885,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
         <v>62</v>
@@ -1920,7 +1911,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1935,18 +1926,18 @@
         <v>67</v>
       </c>
       <c r="J39" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" t="s">
         <v>68</v>
@@ -1967,7 +1958,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1982,18 +1973,18 @@
         <v>72</v>
       </c>
       <c r="J41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D42" t="s">
         <v>73</v>
@@ -2017,7 +2008,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2025,48 +2016,46 @@
         <v>77</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J43" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2078,48 +2067,48 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J48" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2131,23 +2120,23 @@
         <v>11</v>
       </c>
       <c r="J50" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2159,119 +2148,119 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>64</v>
@@ -2280,45 +2269,45 @@
         <v>15</v>
       </c>
       <c r="J61" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C62" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J62" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D63" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63" t="s">
         <v>86</v>
-      </c>
-      <c r="E63" t="s">
-        <v>87</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>64</v>
@@ -2330,41 +2319,41 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D65" t="s">
+        <v>89</v>
+      </c>
+      <c r="E65" t="s">
         <v>90</v>
       </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>91</v>
-      </c>
-      <c r="G65" t="s">
-        <v>92</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>64</v>
@@ -2376,140 +2365,140 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J67" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J69" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2522,7 +2511,7 @@
       </c>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2535,15 +2524,15 @@
       </c>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>44</v>
@@ -2552,27 +2541,27 @@
         <v>15</v>
       </c>
       <c r="J75" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C76" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2584,7 +2573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2596,15 +2585,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H79" t="s">
         <v>56</v>
@@ -2613,21 +2602,21 @@
         <v>15</v>
       </c>
       <c r="J79" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H80" t="s">
         <v>56</v>
@@ -2636,18 +2625,18 @@
         <v>15</v>
       </c>
       <c r="J80" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H81" t="s">
         <v>56</v>
@@ -2656,10 +2645,10 @@
         <v>15</v>
       </c>
       <c r="J81" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2667,7 +2656,7 @@
         <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D82" t="s">
         <v>76</v>
@@ -2679,10 +2668,10 @@
         <v>15</v>
       </c>
       <c r="J82" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2695,7 +2684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2708,12 +2697,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C85" s="1"/>
       <c r="H85" s="1"/>
@@ -2721,15 +2710,15 @@
         <v>11</v>
       </c>
       <c r="J85" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C86" s="1"/>
       <c r="H86" s="1"/>
@@ -2737,15 +2726,15 @@
         <v>11</v>
       </c>
       <c r="J86" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C87" s="1"/>
       <c r="H87" s="1"/>
@@ -2753,15 +2742,15 @@
         <v>11</v>
       </c>
       <c r="J87" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C88" s="1"/>
       <c r="H88" s="1"/>
@@ -2769,10 +2758,10 @@
         <v>11</v>
       </c>
       <c r="J88" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2785,7 +2774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2798,12 +2787,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C91" s="1"/>
       <c r="H91" s="1"/>
@@ -2811,15 +2800,15 @@
         <v>11</v>
       </c>
       <c r="J91" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C92" s="1"/>
       <c r="H92" s="1"/>
@@ -2827,15 +2816,15 @@
         <v>11</v>
       </c>
       <c r="J92" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C93" s="1"/>
       <c r="H93" s="1"/>
@@ -2843,15 +2832,15 @@
         <v>11</v>
       </c>
       <c r="J93" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C94" s="1"/>
       <c r="H94" s="1"/>
@@ -2859,10 +2848,10 @@
         <v>11</v>
       </c>
       <c r="J94" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2875,7 +2864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2888,12 +2877,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C97" s="1"/>
       <c r="H97" s="1"/>
@@ -2901,15 +2890,15 @@
         <v>11</v>
       </c>
       <c r="J97" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C98" s="1"/>
       <c r="H98" s="1"/>
@@ -2917,15 +2906,15 @@
         <v>11</v>
       </c>
       <c r="J98" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C99" s="1"/>
       <c r="H99" s="1"/>
@@ -2933,15 +2922,15 @@
         <v>11</v>
       </c>
       <c r="J99" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C100" s="1"/>
       <c r="H100" s="1"/>
@@ -2949,10 +2938,10 @@
         <v>11</v>
       </c>
       <c r="J100" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2965,7 +2954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2978,7 +2967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2986,8 +2975,8 @@
       <c r="I103" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J102" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J102">
+  <autoFilter ref="A2:J102">
+    <sortState ref="A3:J102">
       <sortCondition ref="A2:A102"/>
     </sortState>
   </autoFilter>
@@ -3001,27 +2990,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="22.26953125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.54296875" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" customWidth="1"/>
-    <col min="10" max="10" width="96.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="96.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3033,7 +3022,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3041,7 +3030,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -3062,10 +3051,10 @@
         <v>7</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3077,7 +3066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3089,7 +3078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3104,7 +3093,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3119,151 +3108,151 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3278,7 +3267,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3293,7 +3282,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3308,7 +3297,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3323,214 +3312,214 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J20" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J24" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C25" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J26" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J28" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C30" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J30" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3546,7 +3535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3558,12 +3547,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -3572,10 +3561,10 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3587,12 +3576,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -3601,18 +3590,18 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D36" s="1"/>
       <c r="H36" t="s">
@@ -3622,15 +3611,15 @@
         <v>15</v>
       </c>
       <c r="J36" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -3639,18 +3628,18 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D38" s="1"/>
       <c r="H38" t="s">
@@ -3660,15 +3649,15 @@
         <v>15</v>
       </c>
       <c r="J38" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -3677,10 +3666,10 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3692,12 +3681,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -3706,10 +3695,10 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3721,12 +3710,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -3735,18 +3724,18 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>13</v>
@@ -3761,15 +3750,15 @@
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -3778,18 +3767,18 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>18</v>
@@ -3804,15 +3793,15 @@
         <v>15</v>
       </c>
       <c r="J46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -3821,10 +3810,10 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3836,12 +3825,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -3850,35 +3839,35 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C50" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J50" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -3886,35 +3875,35 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C52" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J52" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -3922,35 +3911,35 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C54" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -3958,35 +3947,35 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J56" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -3994,98 +3983,98 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C58" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J58" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J59" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J60" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J61" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C62" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J62" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4098,85 +4087,85 @@
       </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C64" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J64" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J65" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C66" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J67" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C68" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4188,82 +4177,82 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C70" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J71" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C72" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J73" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4275,64 +4264,64 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J77" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J79" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4343,7 +4332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4354,38 +4343,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J82" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J83" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4398,28 +4387,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J85" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1" t="s">
@@ -4429,7 +4418,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4442,12 +4431,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1" t="s">
@@ -4457,7 +4446,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4470,7 +4459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4483,28 +4472,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J91" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1" t="s">
@@ -4514,28 +4503,28 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J93" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1" t="s">
@@ -4545,23 +4534,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J95" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4574,28 +4563,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J97" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="s">
@@ -4605,28 +4594,28 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J99" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1" t="s">
@@ -4636,23 +4625,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J101" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4665,28 +4654,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J102" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J102">
+  <autoFilter ref="A2:J102">
+    <sortState ref="A3:J102">
       <sortCondition ref="A2:A102"/>
     </sortState>
   </autoFilter>

</xml_diff>